<commit_message>
4/26 - office 1
</commit_message>
<xml_diff>
--- a/base/base_inventory.xlsx
+++ b/base/base_inventory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20417"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\__users__\__management__\real_enterprise\base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCCC4D9B-162D-41CD-91BC-E55F01B6922B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEBFE5DB-FFE8-4FBE-9E87-E9C2C969C64D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INVENTORY" sheetId="1" r:id="rId1"/>
@@ -36,21 +36,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="131">
   <si>
     <t>ID</t>
   </si>
@@ -421,9 +412,6 @@
     <t>FREEBIES NAME</t>
   </si>
   <si>
-    <t>DETAILS</t>
-  </si>
-  <si>
     <t>8 Freebies</t>
   </si>
   <si>
@@ -443,6 +431,9 @@
   </si>
   <si>
     <t>FREEBIES SET ID</t>
+  </si>
+  <si>
+    <t>DELL REGULAR 2 / 16</t>
   </si>
 </sst>
 </file>
@@ -631,7 +622,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -651,24 +642,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="23">
     <dxf>
       <font>
         <b/>
@@ -681,41 +666,36 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color theme="1"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF5B9BD5"/>
-          <bgColor rgb="FF5B9BD5"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <b/>
       </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFDDEBF7"/>
-          <bgColor rgb="FFDDEBF7"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -798,13 +778,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color rgb="FF9BC2E6"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color rgb="FF9BC2E6"/>
         </left>
@@ -820,21 +793,35 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFDDEBF7"/>
+          <bgColor rgb="FFDDEBF7"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF9BC2E6"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -848,27 +835,17 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FFFFFFFF"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF5B9BD5"/>
+          <bgColor rgb="FF5B9BD5"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -928,24 +905,30 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D7793D7E-998E-4340-B665-58A624CA35C1}" name="_TBL_INVENTORY" displayName="_TBL_INVENTORY" ref="B2:H112" totalsRowShown="0" dataDxfId="24">
-  <autoFilter ref="B2:H112" xr:uid="{D7793D7E-998E-4340-B665-58A624CA35C1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D7793D7E-998E-4340-B665-58A624CA35C1}" name="_TBL_INVENTORY" displayName="_TBL_INVENTORY" ref="B2:H112" totalsRowShown="0" dataDxfId="22">
+  <autoFilter ref="B2:H112" xr:uid="{D7793D7E-998E-4340-B665-58A624CA35C1}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Add Ons"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{56F98167-A797-429F-9D5B-36A31BD611C6}" name="ID" dataDxfId="23">
+    <tableColumn id="1" xr3:uid="{56F98167-A797-429F-9D5B-36A31BD611C6}" name="ID" dataDxfId="21">
       <calculatedColumnFormula array="1">IF(_TBL_INVENTORY[[#This Row],[NAME]]="", "", INDEX(_TBL_INVENTORY[ID],ROW()-ROW(_TBL_INVENTORY[#Headers]))+1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{A455ACF3-9F4A-4528-B37E-016C6CF99C23}" name="NAME" dataDxfId="22">
+    <tableColumn id="2" xr3:uid="{A455ACF3-9F4A-4528-B37E-016C6CF99C23}" name="NAME" dataDxfId="20">
       <calculatedColumnFormula>_xlfn.TEXTJOIN(" ", TRUE, _TBL_INVENTORY[[#This Row],[BRAND]], _TBL_INVENTORY[[#This Row],[CODE]], _TBL_INVENTORY[[#This Row],[VARIANT]], _TBL_INVENTORY[[#This Row],[SPECS]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{7F0CEBD5-4CE4-433D-8A6E-C1E342775294}" name="TYPE" dataDxfId="21">
+    <tableColumn id="3" xr3:uid="{7F0CEBD5-4CE4-433D-8A6E-C1E342775294}" name="TYPE" dataDxfId="19">
       <calculatedColumnFormula array="1">_xlfn._xlws.FILTER(_TBL_INVENTORY_TYPE[NAME], TRUE, "NO DATA")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{02050A77-D5F0-4668-A774-8302CA0A05E5}" name="BRAND" dataDxfId="20">
+    <tableColumn id="4" xr3:uid="{02050A77-D5F0-4668-A774-8302CA0A05E5}" name="BRAND" dataDxfId="18">
       <calculatedColumnFormula array="1">_TBL_INVENTORY_TYPE[NAME]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{D579966A-DEF4-4F23-9EB0-F455C229761E}" name="CODE" dataDxfId="19"/>
-    <tableColumn id="7" xr3:uid="{8FE9C4CC-BA2B-4D29-9D5C-62A59FD184A3}" name="VARIANT" dataDxfId="18"/>
-    <tableColumn id="6" xr3:uid="{BAEB2A07-6602-4B05-9C73-7A790A4A0E22}" name="SPECS" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{D579966A-DEF4-4F23-9EB0-F455C229761E}" name="CODE" dataDxfId="17"/>
+    <tableColumn id="7" xr3:uid="{8FE9C4CC-BA2B-4D29-9D5C-62A59FD184A3}" name="VARIANT" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{BAEB2A07-6602-4B05-9C73-7A790A4A0E22}" name="SPECS" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -955,7 +938,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D441CA89-0936-4083-8D2D-762AEB7CF49D}" name="_TBL_DATES" displayName="_TBL_DATES" ref="B2:F10" totalsRowShown="0">
   <autoFilter ref="B2:F10" xr:uid="{D441CA89-0936-4083-8D2D-762AEB7CF49D}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{E2B553E0-CAEF-4A90-A625-C81B383B0525}" name="DATE" dataDxfId="7">
+    <tableColumn id="1" xr3:uid="{E2B553E0-CAEF-4A90-A625-C81B383B0525}" name="DATE" dataDxfId="4">
       <calculatedColumnFormula>TODAY()</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{3977A4BE-9ECC-428A-AD33-9D57D8915200}" name="START_DATE"/>
@@ -983,35 +966,32 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{27BD5B1B-DBD6-4D7D-B660-C8A0AB832FA9}" name="_TBL_PRODUCT_CATALOG" displayName="_TBL_PRODUCT_CATALOG" ref="B2:C33" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowBorderDxfId="5" tableBorderDxfId="6" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{27BD5B1B-DBD6-4D7D-B660-C8A0AB832FA9}" name="_TBL_FREEBIES_CATALOG" displayName="_TBL_FREEBIES_CATALOG" ref="B2:C33" totalsRowShown="0" headerRowDxfId="14" dataDxfId="12" headerRowBorderDxfId="13" tableBorderDxfId="11" totalsRowBorderDxfId="10">
   <autoFilter ref="B2:C33" xr:uid="{27BD5B1B-DBD6-4D7D-B660-C8A0AB832FA9}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{7436F674-F68B-4607-8BF6-E1495AFBF453}" name="FREEBIES SET ID" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{C920ECEE-E736-4E62-8DFA-A29F851BF4AE}" name="INVENTORY ID" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{7436F674-F68B-4607-8BF6-E1495AFBF453}" name="FREEBIES SET ID" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{C920ECEE-E736-4E62-8DFA-A29F851BF4AE}" name="INVENTORY ID" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B3B6E215-0C9E-4DA0-8FC6-7755F7A591EC}" name="_TBL_FREEBIES_SET" displayName="_TBL_FREEBIES_SET" ref="B2:D9" totalsRowCount="1" dataDxfId="16">
-  <autoFilter ref="B2:D8" xr:uid="{B3B6E215-0C9E-4DA0-8FC6-7755F7A591EC}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{32F70E71-6A90-4834-8035-820929A63A88}" name="ID" totalsRowFunction="custom" dataDxfId="15" totalsRowDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B3B6E215-0C9E-4DA0-8FC6-7755F7A591EC}" name="_TBL_FREEBIES_SET" displayName="_TBL_FREEBIES_SET" ref="B2:C9" totalsRowCount="1" dataDxfId="7">
+  <autoFilter ref="B2:C8" xr:uid="{B3B6E215-0C9E-4DA0-8FC6-7755F7A591EC}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{32F70E71-6A90-4834-8035-820929A63A88}" name="ID" totalsRowFunction="custom" dataDxfId="3" totalsRowDxfId="1">
       <totalsRowFormula>_xlfn.CONCAT("COUNT: ", SUBTOTAL(103,_TBL_FREEBIES_SET[ID]))</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{ACE17F3B-3F5B-4373-B364-E484DCAEA00C}" name="FREEBIES NAME" dataDxfId="13" totalsRowDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{3D78DD2F-9502-4479-BC02-D404E7777D9C}" name="DETAILS" dataDxfId="11" totalsRowDxfId="10">
-      <calculatedColumnFormula>IF(_TBL_FREEBIES_SET[[#This Row],[ID]]&lt;&gt;"", GetInventoryList(_TBL_FREEBIES_SET[[#This Row],[ID]]), "")</calculatedColumnFormula>
-    </tableColumn>
+    <tableColumn id="2" xr3:uid="{ACE17F3B-3F5B-4373-B364-E484DCAEA00C}" name="FREEBIES NAME" dataDxfId="2" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{8D17F0C9-2D07-433C-A0FC-345FB0EBC625}" name="_TBL_ADD_ONS" displayName="_TBL_ADD_ONS" ref="B2:D8" totalsRowShown="0">
-  <autoFilter ref="B2:D8" xr:uid="{8D17F0C9-2D07-433C-A0FC-345FB0EBC625}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{8D17F0C9-2D07-433C-A0FC-345FB0EBC625}" name="_TBL_ADD_ONS" displayName="_TBL_ADD_ONS" ref="B2:D47" totalsRowShown="0">
+  <autoFilter ref="B2:D47" xr:uid="{8D17F0C9-2D07-433C-A0FC-345FB0EBC625}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{21597612-61CE-45BC-9EE8-BD8EA0AFAD3C}" name="ID"/>
     <tableColumn id="2" xr3:uid="{712AB32B-16D3-4728-8D3F-55A6FD7B8193}" name="ADD ON NAME"/>
@@ -1050,7 +1030,7 @@
   <autoFilter ref="B3:D16" xr:uid="{059D30F9-D046-4297-B2D5-BC5338888079}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8FD43C8F-1591-412E-BE99-E5A1E14B95C3}" name="ID"/>
-    <tableColumn id="2" xr3:uid="{FE9F0275-0C2B-4FED-9671-794A5EA845F1}" name="NAME" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{FE9F0275-0C2B-4FED-9671-794A5EA845F1}" name="NAME" dataDxfId="6"/>
     <tableColumn id="3" xr3:uid="{28FE780F-BBE9-4B58-AD37-87DA8E77F97E}" name="CODE"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1062,7 +1042,7 @@
   <autoFilter ref="B3:D14" xr:uid="{FEF824DF-57E9-41C7-B4B2-D063ED21B078}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{BB1B283B-D25C-4ADE-980A-2B88D96C5E7C}" name="ID"/>
-    <tableColumn id="2" xr3:uid="{9951A92B-2CA7-435D-ADCB-A39878F2EED5}" name="NAME" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{9951A92B-2CA7-435D-ADCB-A39878F2EED5}" name="NAME" dataDxfId="5"/>
     <tableColumn id="3" xr3:uid="{EF23B0B5-69D7-4593-BCD3-1E27223DDFEC}" name="CODE"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1335,44 +1315,44 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:H112"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C74" sqref="C74"/>
+    <sheetView zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52:C96"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="68.7109375" customWidth="1"/>
+    <col min="3" max="3" width="68.6640625" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1"/>
-    <col min="6" max="6" width="24.140625" customWidth="1"/>
-    <col min="7" max="7" width="25.85546875" customWidth="1"/>
-    <col min="8" max="8" width="30.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" customWidth="1"/>
+    <col min="6" max="6" width="24.109375" customWidth="1"/>
+    <col min="7" max="7" width="25.88671875" customWidth="1"/>
+    <col min="8" max="8" width="30.88671875" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.44140625" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="15" max="17" width="11" customWidth="1"/>
     <col min="20" max="20" width="11" customWidth="1"/>
-    <col min="21" max="21" width="26.5703125" customWidth="1"/>
+    <col min="21" max="21" width="26.5546875" customWidth="1"/>
     <col min="22" max="22" width="11" customWidth="1"/>
-    <col min="25" max="25" width="17.28515625" customWidth="1"/>
-    <col min="26" max="26" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="15.7109375" customWidth="1"/>
-    <col min="29" max="29" width="18.140625" customWidth="1"/>
+    <col min="25" max="25" width="17.33203125" customWidth="1"/>
+    <col min="26" max="26" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.6640625" customWidth="1"/>
+    <col min="29" max="29" width="18.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B1" s="17" t="s">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B1" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-    </row>
-    <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+    </row>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -1395,7 +1375,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4">
         <v>1</v>
       </c>
@@ -1417,7 +1397,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B4" s="4">
         <v>2</v>
       </c>
@@ -1439,7 +1419,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B5" s="4">
         <v>3</v>
       </c>
@@ -1461,7 +1441,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B6" s="4">
         <v>4</v>
       </c>
@@ -1483,7 +1463,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B7" s="4">
         <v>5</v>
       </c>
@@ -1505,7 +1485,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B8" s="4">
         <v>6</v>
       </c>
@@ -1527,7 +1507,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B9" s="4">
         <v>7</v>
       </c>
@@ -1549,7 +1529,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
         <v>8</v>
       </c>
@@ -1571,7 +1551,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B11" s="4">
         <v>9</v>
       </c>
@@ -1593,7 +1573,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B12" s="4">
         <v>10</v>
       </c>
@@ -1615,7 +1595,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B13" s="4">
         <v>11</v>
       </c>
@@ -1637,7 +1617,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B14" s="4">
         <v>12</v>
       </c>
@@ -1659,7 +1639,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B15" s="4">
         <v>13</v>
       </c>
@@ -1681,7 +1661,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B16" s="4">
         <v>14</v>
       </c>
@@ -1703,7 +1683,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B17" s="4">
         <v>15</v>
       </c>
@@ -1725,7 +1705,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B18" s="4">
         <v>16</v>
       </c>
@@ -1747,7 +1727,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B19" s="4">
         <v>17</v>
       </c>
@@ -1769,7 +1749,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B20" s="4">
         <v>18</v>
       </c>
@@ -1791,7 +1771,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B21" s="4">
         <v>19</v>
       </c>
@@ -1813,7 +1793,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B22" s="4">
         <v>20</v>
       </c>
@@ -1835,7 +1815,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B23" s="4">
         <v>21</v>
       </c>
@@ -1857,7 +1837,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B24" s="4">
         <v>22</v>
       </c>
@@ -1879,7 +1859,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B25" s="4">
         <v>23</v>
       </c>
@@ -1901,7 +1881,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B26" s="4">
         <v>24</v>
       </c>
@@ -1923,7 +1903,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B27" s="4">
         <v>25</v>
       </c>
@@ -1945,7 +1925,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B28" s="4">
         <v>26</v>
       </c>
@@ -1967,7 +1947,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B29" s="4">
         <v>27</v>
       </c>
@@ -1989,7 +1969,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B30" s="4">
         <v>28</v>
       </c>
@@ -2011,7 +1991,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B31" s="4">
         <v>29</v>
       </c>
@@ -2033,7 +2013,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B32" s="4">
         <v>30</v>
       </c>
@@ -2055,7 +2035,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B33" s="4">
         <v>31</v>
       </c>
@@ -2077,7 +2057,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B34" s="4">
         <v>32</v>
       </c>
@@ -2099,7 +2079,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B35" s="4">
         <v>33</v>
       </c>
@@ -2121,7 +2101,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B36" s="4">
         <v>34</v>
       </c>
@@ -2143,7 +2123,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B37" s="4">
         <v>35</v>
       </c>
@@ -2165,7 +2145,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B38" s="4">
         <v>36</v>
       </c>
@@ -2187,7 +2167,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B39" s="4">
         <v>37</v>
       </c>
@@ -2209,7 +2189,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B40" s="4">
         <v>38</v>
       </c>
@@ -2231,7 +2211,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B41" s="4">
         <v>39</v>
       </c>
@@ -2251,7 +2231,7 @@
       </c>
       <c r="H41" s="9"/>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B42" s="4">
         <v>40</v>
       </c>
@@ -2271,7 +2251,7 @@
       </c>
       <c r="H42" s="9"/>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B43" s="4">
         <v>41</v>
       </c>
@@ -2289,7 +2269,7 @@
       <c r="G43" s="1"/>
       <c r="H43" s="9"/>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B44" s="4">
         <v>42</v>
       </c>
@@ -2309,7 +2289,7 @@
       </c>
       <c r="H44" s="9"/>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B45" s="4">
         <v>43</v>
       </c>
@@ -2329,7 +2309,7 @@
       </c>
       <c r="H45" s="9"/>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B46" s="4">
         <v>44</v>
       </c>
@@ -2349,7 +2329,7 @@
       </c>
       <c r="H46" s="9"/>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B47" s="4">
         <v>45</v>
       </c>
@@ -2367,7 +2347,7 @@
       <c r="G47" s="1"/>
       <c r="H47" s="9"/>
     </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B48" s="4">
         <v>46</v>
       </c>
@@ -2385,7 +2365,7 @@
       <c r="G48" s="1"/>
       <c r="H48" s="9"/>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B49" s="4">
         <v>47</v>
       </c>
@@ -2405,7 +2385,7 @@
       </c>
       <c r="H49" s="9"/>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B50" s="4">
         <v>48</v>
       </c>
@@ -2425,7 +2405,7 @@
       </c>
       <c r="H50" s="9"/>
     </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B51" s="4">
         <v>49</v>
       </c>
@@ -2443,7 +2423,7 @@
       <c r="G51" s="1"/>
       <c r="H51" s="9"/>
     </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B52" s="4">
         <v>50</v>
       </c>
@@ -2461,7 +2441,7 @@
       <c r="G52" s="1"/>
       <c r="H52" s="9"/>
     </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B53" s="4">
         <v>51</v>
       </c>
@@ -2479,7 +2459,7 @@
       <c r="G53" s="1"/>
       <c r="H53" s="9"/>
     </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B54" s="4">
         <v>52</v>
       </c>
@@ -2497,7 +2477,7 @@
       <c r="G54" s="1"/>
       <c r="H54" s="9"/>
     </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B55" s="4">
         <v>53</v>
       </c>
@@ -2515,7 +2495,7 @@
       <c r="G55" s="1"/>
       <c r="H55" s="9"/>
     </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B56" s="4">
         <v>54</v>
       </c>
@@ -2533,7 +2513,7 @@
       <c r="G56" s="1"/>
       <c r="H56" s="9"/>
     </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B57" s="4">
         <v>55</v>
       </c>
@@ -2551,7 +2531,7 @@
       <c r="G57" s="1"/>
       <c r="H57" s="9"/>
     </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B58" s="4">
         <v>56</v>
       </c>
@@ -2569,7 +2549,7 @@
       <c r="G58" s="1"/>
       <c r="H58" s="9"/>
     </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B59" s="4">
         <v>57</v>
       </c>
@@ -2587,7 +2567,7 @@
       <c r="G59" s="1"/>
       <c r="H59" s="9"/>
     </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B60" s="4">
         <v>58</v>
       </c>
@@ -2605,7 +2585,7 @@
       <c r="G60" s="1"/>
       <c r="H60" s="9"/>
     </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B61" s="4">
         <v>59</v>
       </c>
@@ -2623,7 +2603,7 @@
       <c r="G61" s="1"/>
       <c r="H61" s="9"/>
     </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B62" s="4">
         <v>60</v>
       </c>
@@ -2641,7 +2621,7 @@
       <c r="G62" s="1"/>
       <c r="H62" s="9"/>
     </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B63" s="4">
         <v>61</v>
       </c>
@@ -2659,7 +2639,7 @@
       <c r="G63" s="1"/>
       <c r="H63" s="9"/>
     </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B64" s="4">
         <v>62</v>
       </c>
@@ -2677,7 +2657,7 @@
       <c r="G64" s="1"/>
       <c r="H64" s="9"/>
     </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B65" s="4">
         <v>63</v>
       </c>
@@ -2695,7 +2675,7 @@
       <c r="G65" s="1"/>
       <c r="H65" s="9"/>
     </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B66" s="4">
         <v>64</v>
       </c>
@@ -2713,7 +2693,7 @@
       <c r="G66" s="1"/>
       <c r="H66" s="9"/>
     </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B67" s="4">
         <v>65</v>
       </c>
@@ -2731,7 +2711,7 @@
       <c r="G67" s="1"/>
       <c r="H67" s="9"/>
     </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B68" s="4">
         <v>66</v>
       </c>
@@ -2749,7 +2729,7 @@
       <c r="G68" s="1"/>
       <c r="H68" s="9"/>
     </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B69" s="4">
         <v>67</v>
       </c>
@@ -2767,7 +2747,7 @@
       <c r="G69" s="1"/>
       <c r="H69" s="9"/>
     </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B70" s="4">
         <v>68</v>
       </c>
@@ -2785,7 +2765,7 @@
       <c r="G70" s="1"/>
       <c r="H70" s="9"/>
     </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B71" s="4">
         <v>69</v>
       </c>
@@ -2803,7 +2783,7 @@
       <c r="G71" s="1"/>
       <c r="H71" s="9"/>
     </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B72" s="4">
         <v>70</v>
       </c>
@@ -2821,7 +2801,7 @@
       <c r="G72" s="1"/>
       <c r="H72" s="9"/>
     </row>
-    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B73" s="4">
         <v>71</v>
       </c>
@@ -2839,7 +2819,7 @@
       <c r="G73" s="1"/>
       <c r="H73" s="9"/>
     </row>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B74" s="4">
         <v>72</v>
       </c>
@@ -2857,7 +2837,7 @@
       <c r="G74" s="1"/>
       <c r="H74" s="9"/>
     </row>
-    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B75" s="4">
         <v>73</v>
       </c>
@@ -2875,7 +2855,7 @@
       <c r="G75" s="1"/>
       <c r="H75" s="9"/>
     </row>
-    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B76" s="4">
         <v>74</v>
       </c>
@@ -2893,7 +2873,7 @@
       <c r="G76" s="1"/>
       <c r="H76" s="9"/>
     </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B77" s="4">
         <v>75</v>
       </c>
@@ -2911,7 +2891,7 @@
       <c r="G77" s="1"/>
       <c r="H77" s="9"/>
     </row>
-    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B78" s="4">
         <v>76</v>
       </c>
@@ -2929,7 +2909,7 @@
       <c r="G78" s="1"/>
       <c r="H78" s="9"/>
     </row>
-    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B79" s="4">
         <v>77</v>
       </c>
@@ -2947,7 +2927,7 @@
       <c r="G79" s="1"/>
       <c r="H79" s="9"/>
     </row>
-    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B80" s="4">
         <v>78</v>
       </c>
@@ -2965,7 +2945,7 @@
       <c r="G80" s="1"/>
       <c r="H80" s="9"/>
     </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B81" s="4">
         <v>79</v>
       </c>
@@ -2983,7 +2963,7 @@
       <c r="G81" s="1"/>
       <c r="H81" s="9"/>
     </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B82" s="4">
         <v>80</v>
       </c>
@@ -3001,7 +2981,7 @@
       <c r="G82" s="1"/>
       <c r="H82" s="9"/>
     </row>
-    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B83" s="4">
         <v>81</v>
       </c>
@@ -3019,7 +2999,7 @@
       <c r="G83" s="1"/>
       <c r="H83" s="9"/>
     </row>
-    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B84" s="4">
         <v>82</v>
       </c>
@@ -3037,7 +3017,7 @@
       <c r="G84" s="1"/>
       <c r="H84" s="9"/>
     </row>
-    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B85" s="4">
         <v>83</v>
       </c>
@@ -3055,7 +3035,7 @@
       <c r="G85" s="1"/>
       <c r="H85" s="9"/>
     </row>
-    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B86" s="4">
         <v>84</v>
       </c>
@@ -3073,7 +3053,7 @@
       <c r="G86" s="1"/>
       <c r="H86" s="9"/>
     </row>
-    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B87" s="4">
         <v>85</v>
       </c>
@@ -3091,7 +3071,7 @@
       <c r="G87" s="1"/>
       <c r="H87" s="9"/>
     </row>
-    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B88" s="4">
         <v>86</v>
       </c>
@@ -3109,7 +3089,7 @@
       <c r="G88" s="1"/>
       <c r="H88" s="9"/>
     </row>
-    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B89" s="4">
         <v>87</v>
       </c>
@@ -3127,7 +3107,7 @@
       <c r="G89" s="1"/>
       <c r="H89" s="9"/>
     </row>
-    <row r="90" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B90" s="4">
         <v>88</v>
       </c>
@@ -3145,7 +3125,7 @@
       <c r="G90" s="1"/>
       <c r="H90" s="9"/>
     </row>
-    <row r="91" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B91" s="4">
         <v>89</v>
       </c>
@@ -3163,7 +3143,7 @@
       <c r="G91" s="1"/>
       <c r="H91" s="9"/>
     </row>
-    <row r="92" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B92" s="4">
         <v>90</v>
       </c>
@@ -3181,7 +3161,7 @@
       <c r="G92" s="1"/>
       <c r="H92" s="9"/>
     </row>
-    <row r="93" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B93" s="4">
         <v>91</v>
       </c>
@@ -3199,7 +3179,7 @@
       <c r="G93" s="1"/>
       <c r="H93" s="9"/>
     </row>
-    <row r="94" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B94" s="4">
         <v>92</v>
       </c>
@@ -3217,7 +3197,7 @@
       <c r="G94" s="1"/>
       <c r="H94" s="9"/>
     </row>
-    <row r="95" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B95" s="4">
         <v>93</v>
       </c>
@@ -3235,7 +3215,7 @@
       <c r="G95" s="1"/>
       <c r="H95" s="9"/>
     </row>
-    <row r="96" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B96" s="4">
         <v>94</v>
       </c>
@@ -3253,7 +3233,7 @@
       <c r="G96" s="1"/>
       <c r="H96" s="9"/>
     </row>
-    <row r="97" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B97" s="4">
         <v>95</v>
       </c>
@@ -3275,7 +3255,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="98" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B98" s="4">
         <v>96</v>
       </c>
@@ -3295,7 +3275,7 @@
       </c>
       <c r="H98" s="9"/>
     </row>
-    <row r="99" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B99" s="4">
         <v>97</v>
       </c>
@@ -3313,7 +3293,7 @@
       <c r="G99" s="1"/>
       <c r="H99" s="9"/>
     </row>
-    <row r="100" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B100" s="4">
         <v>98</v>
       </c>
@@ -3331,7 +3311,7 @@
       <c r="G100" s="1"/>
       <c r="H100" s="9"/>
     </row>
-    <row r="101" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B101" s="4">
         <v>99</v>
       </c>
@@ -3349,7 +3329,7 @@
       <c r="G101" s="1"/>
       <c r="H101" s="9"/>
     </row>
-    <row r="102" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B102" s="4">
         <v>100</v>
       </c>
@@ -3367,7 +3347,7 @@
       <c r="G102" s="1"/>
       <c r="H102" s="9"/>
     </row>
-    <row r="103" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B103" s="4">
         <v>101</v>
       </c>
@@ -3385,7 +3365,7 @@
       <c r="G103" s="1"/>
       <c r="H103" s="9"/>
     </row>
-    <row r="104" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B104" s="4">
         <v>102</v>
       </c>
@@ -3403,7 +3383,7 @@
       <c r="G104" s="1"/>
       <c r="H104" s="9"/>
     </row>
-    <row r="105" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B105" s="4">
         <v>103</v>
       </c>
@@ -3421,7 +3401,7 @@
       <c r="G105" s="1"/>
       <c r="H105" s="9"/>
     </row>
-    <row r="106" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B106" s="4">
         <v>104</v>
       </c>
@@ -3439,7 +3419,7 @@
       <c r="G106" s="1"/>
       <c r="H106" s="9"/>
     </row>
-    <row r="107" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B107" s="4"/>
       <c r="C107" t="str">
         <f>_xlfn.TEXTJOIN(" ", TRUE, _TBL_INVENTORY[[#This Row],[BRAND]], _TBL_INVENTORY[[#This Row],[CODE]], _TBL_INVENTORY[[#This Row],[VARIANT]], _TBL_INVENTORY[[#This Row],[SPECS]])</f>
@@ -3451,7 +3431,7 @@
       <c r="G107" s="1"/>
       <c r="H107" s="9"/>
     </row>
-    <row r="108" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B108" s="4"/>
       <c r="C108" t="str">
         <f>_xlfn.TEXTJOIN(" ", TRUE, _TBL_INVENTORY[[#This Row],[BRAND]], _TBL_INVENTORY[[#This Row],[CODE]], _TBL_INVENTORY[[#This Row],[VARIANT]], _TBL_INVENTORY[[#This Row],[SPECS]])</f>
@@ -3463,7 +3443,7 @@
       <c r="G108" s="1"/>
       <c r="H108" s="9"/>
     </row>
-    <row r="109" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B109" s="4"/>
       <c r="C109" t="str">
         <f>_xlfn.TEXTJOIN(" ", TRUE, _TBL_INVENTORY[[#This Row],[BRAND]], _TBL_INVENTORY[[#This Row],[CODE]], _TBL_INVENTORY[[#This Row],[VARIANT]], _TBL_INVENTORY[[#This Row],[SPECS]])</f>
@@ -3475,7 +3455,7 @@
       <c r="G109" s="1"/>
       <c r="H109" s="9"/>
     </row>
-    <row r="110" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B110" s="4"/>
       <c r="C110" t="str">
         <f>_xlfn.TEXTJOIN(" ", TRUE, _TBL_INVENTORY[[#This Row],[BRAND]], _TBL_INVENTORY[[#This Row],[CODE]], _TBL_INVENTORY[[#This Row],[VARIANT]], _TBL_INVENTORY[[#This Row],[SPECS]])</f>
@@ -3487,7 +3467,7 @@
       <c r="G110" s="1"/>
       <c r="H110" s="9"/>
     </row>
-    <row r="111" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B111" s="4"/>
       <c r="C111" t="str">
         <f>_xlfn.TEXTJOIN(" ", TRUE, _TBL_INVENTORY[[#This Row],[BRAND]], _TBL_INVENTORY[[#This Row],[CODE]], _TBL_INVENTORY[[#This Row],[VARIANT]], _TBL_INVENTORY[[#This Row],[SPECS]])</f>
@@ -3499,7 +3479,7 @@
       <c r="G111" s="1"/>
       <c r="H111" s="9"/>
     </row>
-    <row r="112" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:8" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B112" s="4"/>
       <c r="C112" t="str">
         <f>_xlfn.TEXTJOIN(" ", TRUE, _TBL_INVENTORY[[#This Row],[BRAND]], _TBL_INVENTORY[[#This Row],[CODE]], _TBL_INVENTORY[[#This Row],[VARIANT]], _TBL_INVENTORY[[#This Row],[SPECS]])</f>
@@ -3547,12 +3527,12 @@
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="6" width="33.140625" customWidth="1"/>
+    <col min="2" max="6" width="33.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>17</v>
       </c>
@@ -3569,18 +3549,18 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B3" s="2">
         <f ca="1">TODAY()</f>
-        <v>45770</v>
+        <v>45773</v>
       </c>
       <c r="C3" s="3">
         <f ca="1">TODAY()</f>
-        <v>45770</v>
+        <v>45773</v>
       </c>
       <c r="D3" s="3">
         <f ca="1">TODAY()</f>
-        <v>45770</v>
+        <v>45773</v>
       </c>
       <c r="E3" t="s">
         <v>21</v>
@@ -3590,18 +3570,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" s="2">
         <f t="shared" ref="B4:B10" ca="1" si="0">TODAY()</f>
-        <v>45770</v>
+        <v>45773</v>
       </c>
       <c r="C4" s="3">
         <f ca="1">TODAY()-1</f>
-        <v>45769</v>
+        <v>45772</v>
       </c>
       <c r="D4" s="3">
         <f ca="1">TODAY()-1</f>
-        <v>45769</v>
+        <v>45772</v>
       </c>
       <c r="E4" t="s">
         <v>22</v>
@@ -3611,10 +3591,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>45770</v>
+        <v>45773</v>
       </c>
       <c r="C5" s="3">
         <f ca="1">TODAY()-WEEKDAY(TODAY(),1)+1</f>
@@ -3632,10 +3612,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>45770</v>
+        <v>45773</v>
       </c>
       <c r="C6" s="3">
         <f ca="1">TODAY()-WEEKDAY(TODAY(),1)-6</f>
@@ -3653,10 +3633,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>45770</v>
+        <v>45773</v>
       </c>
       <c r="C7" s="3">
         <f ca="1">EOMONTH(TODAY(),-1)+1</f>
@@ -3674,10 +3654,10 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>45770</v>
+        <v>45773</v>
       </c>
       <c r="C8" s="3">
         <f ca="1">EOMONTH(TODAY(),-2)+1</f>
@@ -3695,10 +3675,10 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>45770</v>
+        <v>45773</v>
       </c>
       <c r="C9" s="3">
         <f ca="1">DATE(YEAR(TODAY()),1,1)</f>
@@ -3716,10 +3696,10 @@
         <v>365</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>45770</v>
+        <v>45773</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -3737,21 +3717,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67B09DFB-FA49-416F-9DAF-E92BF0C096B6}">
-  <dimension ref="B2:G4"/>
+  <sheetPr codeName="Sheet7"/>
+  <dimension ref="B2:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="34.28515625" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.33203125" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -3771,7 +3752,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>119</v>
       </c>
@@ -3779,12 +3760,25 @@
         <v>3990</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>120</v>
       </c>
       <c r="D4">
         <v>3990</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D6">
+        <v>6000</v>
       </c>
     </row>
   </sheetData>
@@ -3805,204 +3799,205 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1B7E052-462E-495F-8FD9-04F1492A8F5C}">
+  <sheetPr codeName="Sheet8"/>
   <dimension ref="B2:C33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C33"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="20" t="s">
-        <v>130</v>
-      </c>
-      <c r="C2" s="20" t="s">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="C2" s="17" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="18">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B3" s="15">
         <v>1</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="15" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="19">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4" s="16">
         <v>1</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="16" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="18">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B5" s="15">
         <v>1</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="15" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="19">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B6" s="16">
         <v>1</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="16" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="18">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B7" s="15">
         <v>1</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="15" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="19">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B8" s="16">
         <v>1</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="16" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="18">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B9" s="15">
         <v>1</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="15" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="19">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B10" s="16">
         <v>1</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="16" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="18">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B11" s="15">
         <v>2</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="15" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B12" s="19">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B12" s="16">
         <v>3</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="16" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B13" s="18">
-        <v>4</v>
-      </c>
-      <c r="C13" s="18" t="s">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B13" s="15">
+        <v>4</v>
+      </c>
+      <c r="C13" s="15" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B14" s="19">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B14" s="16">
         <v>5</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="16" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="18">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B15" s="15">
         <v>5</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="15" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="19"/>
-      <c r="C20" s="19"/>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="19"/>
-      <c r="C22" s="19"/>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="18"/>
-      <c r="C23" s="18"/>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="19"/>
-      <c r="C24" s="19"/>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="18"/>
-      <c r="C25" s="18"/>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="19"/>
-      <c r="C26" s="19"/>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B29" s="18"/>
-      <c r="C29" s="18"/>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B30" s="19"/>
-      <c r="C30" s="19"/>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B31" s="18"/>
-      <c r="C31" s="18"/>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B32" s="19"/>
-      <c r="C32" s="19"/>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B20" s="16"/>
+      <c r="C20" s="16"/>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B24" s="16"/>
+      <c r="C24" s="16"/>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B30" s="16"/>
+      <c r="C30" s="16"/>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B32" s="16"/>
+      <c r="C32" s="16"/>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4014,101 +4009,73 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B33AE20E-7F3B-4B99-B7CE-E7F8F3E42D03}">
-  <dimension ref="B2:D9"/>
+  <sheetPr codeName="Sheet9"/>
+  <dimension ref="B2:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
         <v>122</v>
       </c>
-      <c r="D2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" s="13">
         <v>1</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="D3" s="15" t="e">
-        <f ca="1">IF(_TBL_FREEBIES_SET[[#This Row],[ID]]&lt;&gt;"", GetInventoryList(_TBL_FREEBIES_SET[[#This Row],[ID]]), "")</f>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B4" s="13">
         <v>2</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="D4" s="15" t="e">
-        <f ca="1">IF(_TBL_FREEBIES_SET[[#This Row],[ID]]&lt;&gt;"", GetInventoryList(_TBL_FREEBIES_SET[[#This Row],[ID]]), "")</f>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B5" s="13">
         <v>3</v>
       </c>
       <c r="C5" s="14" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B6" s="13">
+        <v>4</v>
+      </c>
+      <c r="C6" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="D5" s="15" t="e">
-        <f ca="1">IF(_TBL_FREEBIES_SET[[#This Row],[ID]]&lt;&gt;"", GetInventoryList(_TBL_FREEBIES_SET[[#This Row],[ID]]), "")</f>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="13">
-        <v>4</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="D6" s="15" t="e">
-        <f ca="1">IF(_TBL_FREEBIES_SET[[#This Row],[ID]]&lt;&gt;"", GetInventoryList(_TBL_FREEBIES_SET[[#This Row],[ID]]), "")</f>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B7" s="13"/>
       <c r="C7" s="14"/>
-      <c r="D7" s="15" t="str">
-        <f>IF(_TBL_FREEBIES_SET[[#This Row],[ID]]&lt;&gt;"", GetInventoryList(_TBL_FREEBIES_SET[[#This Row],[ID]]), "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B8" s="13"/>
       <c r="C8" s="14"/>
-      <c r="D8" s="15" t="str">
-        <f>IF(_TBL_FREEBIES_SET[[#This Row],[ID]]&lt;&gt;"", GetInventoryList(_TBL_FREEBIES_SET[[#This Row],[ID]]), "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B9" s="13" t="str">
         <f>_xlfn.CONCAT("COUNT: ", SUBTOTAL(103,_TBL_FREEBIES_SET[ID]))</f>
         <v>COUNT: 4</v>
       </c>
       <c r="C9" s="14"/>
-      <c r="D9" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4120,93 +4087,292 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{999EC004-D5A6-4FD2-81AC-503CE05B51A5}">
-  <dimension ref="B2:D8"/>
+  <sheetPr codeName="Sheet10"/>
+  <dimension ref="B2:D47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D2" t="s">
         <v>128</v>
       </c>
-      <c r="D2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>95</v>
+        <v>54</v>
       </c>
       <c r="D3">
         <v>250</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D4">
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D5">
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D6">
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>110</v>
+        <v>58</v>
       </c>
       <c r="D7">
         <v>5000</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="D8">
         <v>300</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C20" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C23" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C24" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C25" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C26" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C27" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C28" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C29" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C30" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="31" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C31" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="32" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C32" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C33" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C34" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C35" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C36" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C37" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C38" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="39" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C39" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="40" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C40" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="41" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C41" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="42" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C42" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="43" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C43" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="44" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C44" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="45" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C45" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="46" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C46" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="47" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C47" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -4223,28 +4389,28 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="17" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -4255,7 +4421,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>1</v>
       </c>
@@ -4263,7 +4429,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>2</v>
       </c>
@@ -4271,7 +4437,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>3</v>
       </c>
@@ -4279,7 +4445,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>4</v>
       </c>
@@ -4287,7 +4453,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>5</v>
       </c>
@@ -4295,7 +4461,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>6</v>
       </c>
@@ -4303,7 +4469,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>7</v>
       </c>
@@ -4311,7 +4477,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>8</v>
       </c>
@@ -4319,7 +4485,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>9</v>
       </c>
@@ -4327,7 +4493,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>10</v>
       </c>
@@ -4335,7 +4501,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>11</v>
       </c>
@@ -4363,26 +4529,26 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.85546875" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" customWidth="1"/>
-    <col min="4" max="4" width="69.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" customWidth="1"/>
+    <col min="4" max="4" width="69.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="17" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -4393,7 +4559,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>1</v>
       </c>
@@ -4404,7 +4570,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>2</v>
       </c>
@@ -4415,7 +4581,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>3</v>
       </c>
@@ -4426,7 +4592,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>4</v>
       </c>
@@ -4437,7 +4603,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>5</v>
       </c>
@@ -4468,20 +4634,20 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="30.28515625" customWidth="1"/>
-    <col min="4" max="4" width="35.140625" customWidth="1"/>
+    <col min="3" max="3" width="30.33203125" customWidth="1"/>
+    <col min="4" max="4" width="35.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="17" t="s">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -4492,7 +4658,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>1</v>
       </c>
@@ -4500,7 +4666,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>2</v>
       </c>
@@ -4508,7 +4674,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>3</v>
       </c>
@@ -4516,7 +4682,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>4</v>
       </c>
@@ -4524,7 +4690,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>5</v>
       </c>
@@ -4532,7 +4698,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>6</v>
       </c>
@@ -4540,7 +4706,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>7</v>
       </c>
@@ -4548,7 +4714,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>8</v>
       </c>
@@ -4556,7 +4722,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>9</v>
       </c>
@@ -4564,16 +4730,16 @@
         <v>99</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C16" s="1"/>
     </row>
   </sheetData>
@@ -4593,23 +4759,23 @@
   <dimension ref="B2:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="30.28515625" customWidth="1"/>
-    <col min="4" max="4" width="35.140625" customWidth="1"/>
+    <col min="3" max="3" width="30.33203125" customWidth="1"/>
+    <col min="4" max="4" width="35.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="17" t="s">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -4620,7 +4786,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>1</v>
       </c>
@@ -4628,7 +4794,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>2</v>
       </c>
@@ -4636,7 +4802,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>3</v>
       </c>
@@ -4644,7 +4810,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>4</v>
       </c>
@@ -4652,7 +4818,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>5</v>
       </c>
@@ -4660,7 +4826,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>6</v>
       </c>
@@ -4668,7 +4834,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>7</v>
       </c>
@@ -4676,7 +4842,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>8</v>
       </c>
@@ -4684,7 +4850,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>9</v>
       </c>
@@ -4692,10 +4858,10 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C14" s="1"/>
     </row>
   </sheetData>

</xml_diff>